<commit_message>
checked the onet item numbers in this table against the truncatedlabels file and highlighted duplicate items across categories for discussion.
</commit_message>
<xml_diff>
--- a/tableitemmatch.xlsx
+++ b/tableitemmatch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuwstout-my.sharepoint.com/personal/stachowskia_uwstout_edu/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuwstout-my.sharepoint.com/personal/stachowskia_uwstout_edu/Documents/00_Spring2022 Research/Job-Demands-Resources/JDRJournalSubmission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="8_{35CA857E-7E5E-491B-9C80-24D3A6485825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{972BF27D-8901-41A3-9D88-4CC1F9AC5CF7}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="8_{35CA857E-7E5E-491B-9C80-24D3A6485825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{330CCAE4-7BC0-46BD-9424-EF5E4C66637D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E1AB594E-F83C-4142-9338-6E89BC953226}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E1AB594E-F83C-4142-9338-6E89BC953226}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="89">
   <si>
     <t>Literature-derived Dimension &amp; Classifcation</t>
   </si>
@@ -249,9 +249,6 @@
   </si>
   <si>
     <t>How much does your job require using your hands to handle, control, or feel objects, tools or controls?</t>
-  </si>
-  <si>
-    <t>How much does your job require kneeling, How much does your job require kneeling, crouching, stooping or crawling?</t>
   </si>
   <si>
     <t>How much does your job require keeping or regaining your balance?</t>
@@ -337,27 +334,28 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <color theme="9" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -389,39 +387,74 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -432,6 +465,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -734,1178 +771,1181 @@
   <dimension ref="A1:O81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.453125" customWidth="1"/>
-    <col min="2" max="2" width="75.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="75.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="11" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="12">
         <v>118</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="12">
         <v>203</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="12">
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="12">
         <v>172</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="12">
         <v>257</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="12">
         <v>342</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="12">
         <v>124</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="12">
         <v>209</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="12">
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="12">
         <v>124</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="12">
         <v>209</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="12">
         <v>294</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="12">
         <v>127</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="12">
         <v>212</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="12">
         <v>297</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="12">
         <v>158</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="12">
         <v>242</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="12">
         <v>328</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="12">
         <v>159</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="12">
         <v>243</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="12">
         <v>329</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="12">
         <v>172</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="12">
         <v>257</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="12">
         <v>342</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="12">
         <v>174</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="12">
         <v>259</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="12">
         <v>344</v>
       </c>
       <c r="O11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="12">
         <v>175</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="12">
         <v>260</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="12">
         <v>345</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="12">
         <v>189</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="12">
         <v>274</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="12">
         <v>359</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="12">
         <v>193</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="12">
         <v>278</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="12">
         <v>363</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="12">
         <v>202</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="12">
         <v>287</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="12">
         <v>372</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="13">
         <v>161</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="13">
         <v>245</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="13">
         <v>331</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="13">
         <v>190</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="13">
         <v>275</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="13">
         <v>360</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="13">
         <v>191</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="13">
         <v>276</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="13">
         <v>361</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="8">
+      <c r="B20" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="14">
         <v>122</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="14">
         <v>207</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="14">
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B21" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="12">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="15">
         <v>137</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="15">
         <v>222</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="15">
         <v>307</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B22" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B23" s="13" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C22" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="12">
         <v>138</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="12">
         <v>223</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="12">
         <v>309</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B24" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="9">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="12">
         <v>139</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="12">
         <v>224</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="12">
         <v>310</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B25" s="13" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="12">
         <v>141</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="12">
         <v>226</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="12">
         <v>312</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B26" s="13" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="12">
         <v>142</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="12">
         <v>227</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="12">
         <v>313</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B27" s="13" t="s">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="12">
         <v>143</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="12">
         <v>228</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="12">
         <v>314</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="13">
         <v>125</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="13">
         <v>210</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="13">
         <v>295</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="13">
         <v>126</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="13">
         <v>211</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="13">
         <v>296</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="12">
         <v>149</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="12">
         <v>233</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="12">
         <v>319</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="12">
         <v>154</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="12">
         <v>238</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="12">
         <v>324</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="12">
         <v>157</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="12">
         <v>241</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="12">
         <v>327</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="12">
         <v>160</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="12">
         <v>244</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="12">
         <v>330</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="12">
         <v>186</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="12">
         <v>271</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="12">
         <v>356</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="12">
         <v>188</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="12">
         <v>273</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="12">
         <v>358</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="12">
         <v>192</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="12">
         <v>277</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="12">
         <v>362</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="12">
         <v>197</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="12">
         <v>282</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="12">
         <v>367</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="12">
         <v>200</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38" s="12">
         <v>285</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="12">
         <v>370</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="12">
         <v>201</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D39" s="12">
         <v>286</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="12">
         <v>371</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B40" s="14" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="12">
         <v>151</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D40" s="12">
         <v>235</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="12">
         <v>321</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="12">
         <v>128</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D41" s="12">
         <v>213</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41" s="12">
         <v>298</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B42" s="15" t="s">
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B43" s="15" t="s">
+      <c r="C42" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B44" s="15" t="s">
+      <c r="C43" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B45" s="15" t="s">
+      <c r="C44" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B46" s="15" t="s">
+      <c r="C45" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B47" s="15" t="s">
+      <c r="C46" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B48" s="15" t="s">
+      <c r="C47" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B49" s="15" t="s">
+      <c r="C48" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B49" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B50" s="15" t="s">
+      <c r="C49" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B51" s="15" t="s">
+      <c r="C50" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B51" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C51" s="12">
         <v>129</v>
       </c>
-      <c r="D51" s="5">
+      <c r="D51" s="12">
         <v>214</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E51" s="12">
         <v>299</v>
       </c>
     </row>
-    <row r="52" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B52" s="15" t="s">
+    <row r="52" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B52" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C52" s="12">
         <v>130</v>
       </c>
-      <c r="D52" s="5">
+      <c r="D52" s="12">
         <v>215</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="12">
         <v>300</v>
       </c>
     </row>
-    <row r="53" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B53" s="15" t="s">
+    <row r="53" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B53" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C53" s="12">
         <v>132</v>
       </c>
-      <c r="D53" s="5">
+      <c r="D53" s="12">
         <v>217</v>
       </c>
-      <c r="E53" s="5">
+      <c r="E53" s="12">
         <v>302</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B54" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C54" s="5">
+    <row r="54" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B54" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="12">
         <v>133</v>
       </c>
-      <c r="D54" s="5">
+      <c r="D54" s="12">
         <v>218</v>
       </c>
-      <c r="E54" s="5">
+      <c r="E54" s="12">
         <v>303</v>
       </c>
     </row>
-    <row r="55" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B55" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" s="5">
+    <row r="55" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B55" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="12">
         <v>134</v>
       </c>
-      <c r="D55" s="5">
+      <c r="D55" s="12">
         <v>219</v>
       </c>
-      <c r="E55" s="5">
+      <c r="E55" s="12">
         <v>304</v>
       </c>
     </row>
-    <row r="56" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B56" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C56" s="5">
+    <row r="56" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B56" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="12">
         <v>136</v>
       </c>
-      <c r="D56" s="5">
+      <c r="D56" s="12">
         <v>221</v>
       </c>
-      <c r="E56" s="5">
+      <c r="E56" s="12">
         <v>306</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B57" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C57" s="5">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C57" s="12">
         <v>137</v>
       </c>
-      <c r="D57" s="5">
+      <c r="D57" s="12">
         <v>222</v>
       </c>
-      <c r="E57" s="5">
+      <c r="E57" s="12">
         <v>307</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B58" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B59" s="15" t="s">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C58" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="12">
         <v>138</v>
       </c>
-      <c r="D59" s="5">
+      <c r="D59" s="12">
         <v>223</v>
       </c>
-      <c r="E59" s="5">
+      <c r="E59" s="12">
         <v>309</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B60" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C60" s="5">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="12">
         <v>139</v>
       </c>
-      <c r="D60" s="5">
+      <c r="D60" s="12">
         <v>224</v>
       </c>
-      <c r="E60" s="5">
+      <c r="E60" s="12">
         <v>310</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B61" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C61" s="5">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" s="12">
         <v>140</v>
       </c>
-      <c r="D61" s="5">
+      <c r="D61" s="12">
         <v>225</v>
       </c>
-      <c r="E61" s="5">
+      <c r="E61" s="12">
         <v>311</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B62" s="15" t="s">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C62" s="12">
         <v>141</v>
       </c>
-      <c r="D62" s="5">
+      <c r="D62" s="12">
         <v>226</v>
       </c>
-      <c r="E62" s="5">
+      <c r="E62" s="12">
         <v>312</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B63" s="15" t="s">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C63" s="12">
         <v>142</v>
       </c>
-      <c r="D63" s="5">
+      <c r="D63" s="12">
         <v>227</v>
       </c>
-      <c r="E63" s="5">
+      <c r="E63" s="12">
         <v>313</v>
       </c>
     </row>
-    <row r="64" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B64" s="15" t="s">
+    <row r="64" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B64" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C64" s="12">
         <v>143</v>
       </c>
-      <c r="D64" s="5">
+      <c r="D64" s="12">
         <v>228</v>
       </c>
-      <c r="E64" s="5">
+      <c r="E64" s="12">
         <v>314</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B65" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C65" s="5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65" s="12">
         <v>144</v>
       </c>
-      <c r="D65" s="5">
+      <c r="D65" s="12">
         <v>229</v>
       </c>
-      <c r="E65" s="5">
+      <c r="E65" s="12">
         <v>315</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B66" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C66" s="5">
+    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B66" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C66" s="12">
         <v>146</v>
       </c>
-      <c r="D66" s="5">
+      <c r="D66" s="12">
         <v>230</v>
       </c>
-      <c r="E66" s="5">
+      <c r="E66" s="12">
         <v>316</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B67" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C67" s="5">
+    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B67" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" s="12">
         <v>147</v>
       </c>
-      <c r="D67" s="5">
+      <c r="D67" s="12">
         <v>231</v>
       </c>
-      <c r="E67" s="5">
+      <c r="E67" s="12">
         <v>317</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B68" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C68" s="5">
+    <row r="68" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B68" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="12">
         <v>148</v>
       </c>
-      <c r="D68" s="5">
+      <c r="D68" s="12">
         <v>232</v>
       </c>
-      <c r="E68" s="5">
+      <c r="E68" s="12">
         <v>318</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B69" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C69" s="5">
+    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B69" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C69" s="12">
         <v>177</v>
       </c>
-      <c r="D69" s="5">
+      <c r="D69" s="12">
         <v>262</v>
       </c>
-      <c r="E69" s="5">
+      <c r="E69" s="12">
         <v>347</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B70" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C70" s="5">
+    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B70" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C70" s="12">
         <v>180</v>
       </c>
-      <c r="D70" s="5">
+      <c r="D70" s="12">
         <v>265</v>
       </c>
-      <c r="E70" s="5">
+      <c r="E70" s="12">
         <v>350</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B71" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C71" s="5">
+    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B71" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71" s="12">
         <v>182</v>
       </c>
-      <c r="D71" s="5">
+      <c r="D71" s="12">
         <v>267</v>
       </c>
-      <c r="E71" s="5">
+      <c r="E71" s="12">
         <v>352</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B72" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C72" s="5">
+    <row r="72" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B72" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C72" s="12">
         <v>181</v>
       </c>
-      <c r="D72" s="5">
+      <c r="D72" s="12">
         <v>266</v>
       </c>
-      <c r="E72" s="5">
+      <c r="E72" s="12">
         <v>351</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B73" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C73" s="5">
+    <row r="73" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B73" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C73" s="12">
         <v>183</v>
       </c>
-      <c r="D73" s="5">
+      <c r="D73" s="12">
         <v>286</v>
       </c>
-      <c r="E73" s="5">
+      <c r="E73" s="12">
         <v>353</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>54</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C74" s="4">
+      <c r="C74" s="13">
         <v>127</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D74" s="13">
         <v>212</v>
       </c>
-      <c r="E74" s="4">
+      <c r="E74" s="13">
         <v>297</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>55</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C75" s="12">
         <v>150</v>
       </c>
-      <c r="D75" s="5">
+      <c r="D75" s="12">
         <v>234</v>
       </c>
-      <c r="E75" s="5">
+      <c r="E75" s="12">
         <v>320</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C76" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D76" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E76" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="C76" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E76" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C77" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E77" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C77" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E77" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C78" s="12">
         <v>155</v>
       </c>
-      <c r="D78" s="5">
+      <c r="D78" s="12">
         <v>239</v>
       </c>
-      <c r="E78" s="5">
+      <c r="E78" s="12">
         <v>325</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C79" s="12">
         <v>199</v>
       </c>
-      <c r="D79" s="5">
+      <c r="D79" s="12">
         <v>284</v>
       </c>
-      <c r="E79" s="5">
+      <c r="E79" s="12">
         <v>369</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>61</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C80" s="12">
         <v>120</v>
       </c>
-      <c r="D80" s="5">
+      <c r="D80" s="12">
         <v>205</v>
       </c>
-      <c r="E80" s="5">
+      <c r="E80" s="12">
         <v>290</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C81" s="12">
         <v>121</v>
       </c>
-      <c r="D81" s="5">
+      <c r="D81" s="12">
         <v>206</v>
       </c>
-      <c r="E81" s="5">
+      <c r="E81" s="12">
         <v>291</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28:B29">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>